<commit_message>
Corrida | SFE-VIPA | 2026-01-26 10:16:33.470083
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-VIPA_out.xlsx
+++ b/web_ces/indicadores/SFE-VIPA_out.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Fecha</t>
   </si>
   <si>
-    <t xml:space="preserve">23/01/2026</t>
+    <t xml:space="preserve">26/01/2026</t>
   </si>
   <si>
     <t xml:space="preserve">Usuario</t>
@@ -1993,7 +1993,7 @@
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9" t="n">
-        <v>0.529276541359668</v>
+        <v>0.528158354151267</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -2051,7 +2051,7 @@
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" t="n">
-        <v>0.251437333373035</v>
+        <v>0.250930804252194</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -2121,7 +2121,7 @@
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18" t="n">
-        <v>0.00363269001754134</v>
+        <v>0.00342330347620284</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -2151,7 +2151,7 @@
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20" t="n">
-        <v>0.000628280925887285</v>
+        <v>0.000585001404445339</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -24408,7 +24408,7 @@
         <v>462</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>-0.0477220677466478</v>
+        <v>-0.0478542398979588</v>
       </c>
     </row>
     <row r="6">
@@ -24416,7 +24416,7 @@
         <v>463</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>-0.0154009077115267</v>
+        <v>-0.0160441324839736</v>
       </c>
     </row>
     <row r="7">
@@ -24424,7 +24424,7 @@
         <v>464</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.0160890893271778</v>
+        <v>0.0149292879196663</v>
       </c>
     </row>
     <row r="8">
@@ -24432,7 +24432,7 @@
         <v>465</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.0643475287452908</v>
+        <v>0.0630595587787394</v>
       </c>
     </row>
     <row r="9">
@@ -24440,7 +24440,7 @@
         <v>466</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.0945213487785438</v>
+        <v>0.0933184843914822</v>
       </c>
     </row>
     <row r="10">
@@ -24448,7 +24448,7 @@
         <v>467</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.123124597113992</v>
+        <v>0.122865061752744</v>
       </c>
     </row>
     <row r="11">
@@ -24456,7 +24456,7 @@
         <v>468</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.201413648434289</v>
+        <v>0.202048344046742</v>
       </c>
     </row>
     <row r="12">
@@ -24464,7 +24464,7 @@
         <v>469</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.298995533409315</v>
+        <v>0.299654860478861</v>
       </c>
     </row>
     <row r="13">
@@ -24472,7 +24472,7 @@
         <v>470</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.399714037723741</v>
+        <v>0.39999826178078</v>
       </c>
     </row>
     <row r="14">
@@ -24480,7 +24480,7 @@
         <v>471</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.501435273363407</v>
+        <v>0.500929939464785</v>
       </c>
     </row>
     <row r="15">
@@ -24488,7 +24488,7 @@
         <v>472</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.529276541359668</v>
+        <v>0.528158354151267</v>
       </c>
     </row>
     <row r="16">
@@ -24496,7 +24496,7 @@
         <v>473</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.508552051401244</v>
+        <v>0.507748232067635</v>
       </c>
     </row>
     <row r="17">
@@ -24504,7 +24504,7 @@
         <v>474</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.503255910956012</v>
+        <v>0.503408591447799</v>
       </c>
     </row>
     <row r="18">
@@ -24512,7 +24512,7 @@
         <v>475</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.49075818891676</v>
+        <v>0.491708087986363</v>
       </c>
     </row>
     <row r="19">
@@ -24520,7 +24520,7 @@
         <v>476</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>0.468976641452422</v>
+        <v>0.469696469278399</v>
       </c>
     </row>
     <row r="20">
@@ -24528,7 +24528,7 @@
         <v>477</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0.446328603235106</v>
+        <v>0.446061340586605</v>
       </c>
     </row>
     <row r="21">
@@ -24536,7 +24536,7 @@
         <v>478</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>0.417070057394643</v>
+        <v>0.416416786526705</v>
       </c>
     </row>
     <row r="22">
@@ -24544,7 +24544,7 @@
         <v>479</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>0.390569313166496</v>
+        <v>0.390041349692768</v>
       </c>
     </row>
     <row r="23">
@@ -24552,7 +24552,7 @@
         <v>480</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.340864234946923</v>
+        <v>0.339747966985458</v>
       </c>
     </row>
     <row r="24">
@@ -24580,237 +24580,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
-    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
-    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BAB046-E941-4482-9038-4109E5AE7D94}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65855B10-8257-4E25-8181-BB1060A05724}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1A6CD66-4B1C-4DE7-9435-10F655F2D976}"/>
 </file>
</xml_diff>